<commit_message>
License and Readme added
</commit_message>
<xml_diff>
--- a/COVID19.xlsx
+++ b/COVID19.xlsx
@@ -461,58 +461,58 @@
                   <c:v>1564</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1564</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -621,58 +621,58 @@
                   <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1550</c:v>
+                  <c:v>1795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,11 +689,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="75497472"/>
-        <c:axId val="75499008"/>
+        <c:axId val="64987520"/>
+        <c:axId val="64989056"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75497472"/>
+        <c:axId val="64987520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,14 +703,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75499008"/>
+        <c:crossAx val="64989056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75499008"/>
+        <c:axId val="64989056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,7 +740,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75497472"/>
+        <c:crossAx val="64987520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1041,11 +1041,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78204288"/>
-        <c:axId val="78548992"/>
+        <c:axId val="68700032"/>
+        <c:axId val="68701568"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78204288"/>
+        <c:axId val="68700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,14 +1055,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78548992"/>
+        <c:crossAx val="68701568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="78548992"/>
+        <c:axId val="68701568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1078,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="78204288"/>
+        <c:crossAx val="68700032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1385,58 +1385,58 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1689,7 +1689,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2365,11 +2365,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="79065472"/>
-        <c:axId val="79067008"/>
+        <c:axId val="124748928"/>
+        <c:axId val="124750464"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="79065472"/>
+        <c:axId val="124748928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,14 +2379,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79067008"/>
+        <c:crossAx val="124750464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="79067008"/>
+        <c:axId val="124750464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2402,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79065472"/>
+        <c:crossAx val="124748928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2994,10 +2994,10 @@
                   <c:v>66.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>133.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>-200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3298,10 +3298,10 @@
                   <c:v>14.123006833712983</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>8.1632653061224492</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>-200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3366,11 +3366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66986752"/>
-        <c:axId val="75527680"/>
+        <c:axId val="125127296"/>
+        <c:axId val="125133184"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="66986752"/>
+        <c:axId val="125127296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3380,14 +3380,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75527680"/>
+        <c:crossAx val="125133184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75527680"/>
+        <c:axId val="125133184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3397,7 +3397,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66986752"/>
+        <c:crossAx val="125127296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3834,10 +3834,10 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5161,28 +5161,26 @@
         <v>43916</v>
       </c>
       <c r="C30">
-        <f>C29</f>
-        <v>1564</v>
+        <v>1819</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="E30">
         <f t="shared" si="7"/>
-        <v>-200</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:F47" si="8">F29</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H30">
         <f t="shared" si="4"/>
-        <v>-200</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="I30">
         <f t="shared" si="5"/>
@@ -5197,7 +5195,7 @@
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -5209,28 +5207,28 @@
         <v>43917</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:C47" si="9">C30</f>
-        <v>1564</v>
+        <f t="shared" ref="C31:C47" si="8">C30</f>
+        <v>1819</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E31" t="e">
+      <c r="E31">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>-200</v>
       </c>
       <c r="F31">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" ref="F30:F47" si="9">F30</f>
+        <v>19</v>
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" t="e">
+      <c r="H31">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>-200</v>
       </c>
       <c r="I31">
         <f t="shared" si="5"/>
@@ -5245,7 +5243,7 @@
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -5257,8 +5255,8 @@
         <v>43918</v>
       </c>
       <c r="C32">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
@@ -5269,8 +5267,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F32">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
@@ -5293,7 +5291,7 @@
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -5305,8 +5303,8 @@
         <v>43919</v>
       </c>
       <c r="C33">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
@@ -5317,8 +5315,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F33">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G33">
         <f t="shared" si="3"/>
@@ -5341,7 +5339,7 @@
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -5353,8 +5351,8 @@
         <v>43920</v>
       </c>
       <c r="C34">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
@@ -5365,8 +5363,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F34">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G34">
         <f t="shared" si="3"/>
@@ -5389,7 +5387,7 @@
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -5401,8 +5399,8 @@
         <v>43921</v>
       </c>
       <c r="C35">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
@@ -5413,8 +5411,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F35">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G35">
         <f t="shared" si="3"/>
@@ -5437,7 +5435,7 @@
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -5449,8 +5447,8 @@
         <v>43922</v>
       </c>
       <c r="C36">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
@@ -5461,8 +5459,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F36">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G36">
         <f t="shared" si="3"/>
@@ -5485,7 +5483,7 @@
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -5497,8 +5495,8 @@
         <v>43923</v>
       </c>
       <c r="C37">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
@@ -5509,8 +5507,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F37">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G37">
         <f t="shared" si="3"/>
@@ -5533,7 +5531,7 @@
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -5545,8 +5543,8 @@
         <v>43924</v>
       </c>
       <c r="C38">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
@@ -5557,8 +5555,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F38">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G38">
         <f t="shared" si="3"/>
@@ -5581,7 +5579,7 @@
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -5593,8 +5591,8 @@
         <v>43925</v>
       </c>
       <c r="C39">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
@@ -5605,8 +5603,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F39">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G39">
         <f t="shared" si="3"/>
@@ -5629,7 +5627,7 @@
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -5641,8 +5639,8 @@
         <v>43926</v>
       </c>
       <c r="C40">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
@@ -5653,8 +5651,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F40">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G40">
         <f t="shared" si="3"/>
@@ -5677,7 +5675,7 @@
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -5689,8 +5687,8 @@
         <v>43927</v>
       </c>
       <c r="C41">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
@@ -5701,8 +5699,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F41">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G41">
         <f t="shared" si="3"/>
@@ -5725,7 +5723,7 @@
       </c>
       <c r="L41">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -5737,8 +5735,8 @@
         <v>43928</v>
       </c>
       <c r="C42">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D42">
         <f t="shared" si="2"/>
@@ -5749,8 +5747,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F42">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G42">
         <f t="shared" si="3"/>
@@ -5773,7 +5771,7 @@
       </c>
       <c r="L42">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -5785,8 +5783,8 @@
         <v>43929</v>
       </c>
       <c r="C43">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D43">
         <f t="shared" si="2"/>
@@ -5797,8 +5795,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F43">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G43">
         <f t="shared" si="3"/>
@@ -5821,7 +5819,7 @@
       </c>
       <c r="L43">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -5833,8 +5831,8 @@
         <v>43930</v>
       </c>
       <c r="C44">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D44">
         <f t="shared" si="2"/>
@@ -5845,8 +5843,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F44">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G44">
         <f t="shared" si="3"/>
@@ -5869,7 +5867,7 @@
       </c>
       <c r="L44">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -5881,8 +5879,8 @@
         <v>43931</v>
       </c>
       <c r="C45">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D45">
         <f t="shared" si="2"/>
@@ -5893,8 +5891,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F45">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G45">
         <f t="shared" si="3"/>
@@ -5917,7 +5915,7 @@
       </c>
       <c r="L45">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -5929,8 +5927,8 @@
         <v>43932</v>
       </c>
       <c r="C46">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D46">
         <f t="shared" si="2"/>
@@ -5941,8 +5939,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F46">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G46">
         <f t="shared" si="3"/>
@@ -5965,7 +5963,7 @@
       </c>
       <c r="L46">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -5977,8 +5975,8 @@
         <v>43933</v>
       </c>
       <c r="C47">
-        <f t="shared" si="9"/>
-        <v>1564</v>
+        <f t="shared" si="8"/>
+        <v>1819</v>
       </c>
       <c r="D47">
         <f t="shared" si="2"/>
@@ -5989,8 +5987,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F47">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G47">
         <f t="shared" si="3"/>
@@ -6013,7 +6011,7 @@
       </c>
       <c r="L47">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exponential rate started of at under x^2.0 but reached x^2.323
</commit_message>
<xml_diff>
--- a/COVID19.xlsx
+++ b/COVID19.xlsx
@@ -3961,868 +3961,868 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9245776533796644</c:v>
+                  <c:v>5.0037163204530648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.513502532843187</c:v>
+                  <c:v>12.833723394957733</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.251465064166357</c:v>
+                  <c:v>25.037177015568354</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.516414917319047</c:v>
+                  <c:v>42.044318762978683</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61.62371493874938</c:v>
+                  <c:v>64.216311203530324</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.846708163528803</c:v>
+                  <c:v>91.867679574283258</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119.42822291671121</c:v>
+                  <c:v>125.27893125087172</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>156.58774563947284</c:v>
+                  <c:v>164.70445617828545</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>199.52623149688802</c:v>
+                  <c:v>210.37784397664763</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>248.42950605272017</c:v>
+                  <c:v>262.51565509502507</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>303.47076950560364</c:v>
+                  <c:v>321.32020440839761</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>364.81249970724673</c:v>
+                  <c:v>386.98168153831477</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>432.60793594507902</c:v>
+                  <c:v>459.67980760799372</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>507.00226068959734</c:v>
+                  <c:v>539.58515733349998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>588.1335577584814</c:v>
+                  <c:v>626.86023290890432</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>676.13360113393901</c:v>
+                  <c:v>721.66034956646433</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>771.12851296924589</c:v>
+                  <c:v>824.13437543063276</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>873.2393188170181</c:v>
+                  <c:v>934.42535671737608</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>982.58242089263194</c:v>
+                  <c:v>1052.6710513676792</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1099.2700051062543</c:v>
+                  <c:v>1179.0043885929597</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1223.4103939473741</c:v>
+                  <c:v>1313.5538677734057</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1355.108354635134</c:v>
+                  <c:v>1456.4439071926699</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1494.465369961227</c:v>
+                  <c:v>1607.7951508896153</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1641.5798777523532</c:v>
+                  <c:v>1767.7247402429612</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1796.5474837318832</c:v>
+                  <c:v>1936.3465556296376</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1959.4611516717455</c:v>
+                  <c:v>2113.771432509051</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2130.4113740298362</c:v>
+                  <c:v>2300.1073555108433</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2309.4863257178449</c:v>
+                  <c:v>2495.4596334901012</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2496.7720032049629</c:v>
+                  <c:v>2699.931058023868</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2692.3523508091321</c:v>
+                  <c:v>2913.6220474276256</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2896.3093757400966</c:v>
+                  <c:v>3136.6307780492934</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3108.7232532236912</c:v>
+                  <c:v>3369.0533043356754</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3329.6724228433168</c:v>
+                  <c:v>3610.9836689495814</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3559.2336770741695</c:v>
+                  <c:v>3862.5140040363508</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3797.4822428522434</c:v>
+                  <c:v>4123.7346245886538</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4044.4918569077827</c:v>
+                  <c:v>4394.7341147325396</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4300.3348354987693</c:v>
+                  <c:v>4675.5994076519155</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4565.0821390994806</c:v>
+                  <c:v>4966.4158597783535</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4838.8034325315484</c:v>
+                  <c:v>5267.2673197969425</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5121.5671409661954</c:v>
+                  <c:v>5578.2361929530007</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5413.4405021768116</c:v>
+                  <c:v>5899.403501088379</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5714.4896153773952</c:v>
+                  <c:v>6230.8489387876498</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6024.779486945642</c:v>
+                  <c:v>6572.6509259720251</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6344.3740732964943</c:v>
+                  <c:v>6924.8866572428878</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6673.3363211442738</c:v>
+                  <c:v>7287.6321482443909</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7011.7282053664685</c:v>
+                  <c:v>7660.9622792873633</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7359.6107646608343</c:v>
+                  <c:v>8044.9508364516587</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7717.0441351681975</c:v>
+                  <c:v>8439.6705503631802</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8084.0875822169628</c:v>
+                  <c:v>8845.19313282236</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8460.7995303299267</c:v>
+                  <c:v>9261.5893114445098</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>8847.2375916215024</c:v>
+                  <c:v>9688.9288624571036</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>9243.4585927010576</c:v>
+                  <c:v>10127.280641786332</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9649.5186001882612</c:v>
+                  <c:v>10576.712614553002</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>10065.472944936637</c:v>
+                  <c:v>11037.291883087411</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>10491.37624505321</c:v>
+                  <c:v>11509.084713563765</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>10927.282427795029</c:v>
+                  <c:v>11992.156561345526</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>11373.244750415992</c:v>
+                  <c:v>12486.572095126221</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>11829.315820032152</c:v>
+                  <c:v>12992.395219942753</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>12295.547612567134</c:v>
+                  <c:v>13509.689099132138</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>12771.991490835913</c:v>
+                  <c:v>14038.516175297907</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>13258.698221818851</c:v>
+                  <c:v>14578.938190345483</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>13755.717993175651</c:v>
+                  <c:v>15131.016204643307</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>14263.100429043665</c:v>
+                  <c:v>15694.810615360644</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>14780.894605163148</c:v>
+                  <c:v>16270.381174030408</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15309.149063367115</c:v>
+                  <c:v>16857.787003380745</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>15847.911825473058</c:v>
+                  <c:v>17457.086613477069</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>16397.230406608742</c:v>
+                  <c:v>18068.337917212506</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>16957.15182800372</c:v>
+                  <c:v>18691.59824518222</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>17527.72262927581</c:v>
+                  <c:v>19326.924359975237</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>18108.988880238638</c:v>
+                  <c:v>19974.372469914062</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>18700.996192256236</c:v>
+                  <c:v>20633.998242271638</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>19303.789729167664</c:v>
+                  <c:v>21305.856815991738</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>19917.414217804115</c:v>
+                  <c:v>21990.0028139391</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>20541.913958118472</c:v>
+                  <c:v>22686.490354701677</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>21177.332832947341</c:v>
+                  <c:v>23395.373063968567</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>21823.714317422939</c:v>
+                  <c:v>24116.704085502843</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>22481.101488051965</c:v>
+                  <c:v>24850.536091729886</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>23149.537031478074</c:v>
+                  <c:v>25596.921293959309</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>23829.063252941665</c:v>
+                  <c:v>26355.911452257031</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>24519.722084452245</c:v>
+                  <c:v>27127.557884984755</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>25221.555092685732</c:v>
+                  <c:v>27911.911478020902</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>25934.603486620148</c:v>
+                  <c:v>28709.022693678744</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>26658.908124920301</c:v>
+                  <c:v>29518.94157933387</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27394.509523083809</c:v>
+                  <c:v>30341.717775775051</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>28141.447860357657</c:v>
+                  <c:v>31177.40052528942</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>28899.762986436941</c:v>
+                  <c:v>32026.038679494508</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>29669.494427952748</c:v>
+                  <c:v>32887.680706927225</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>30450.681394760803</c:v>
+                  <c:v>33762.374700399829</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>31243.362786037218</c:v>
+                  <c:v>34650.168384133904</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>32047.577196189912</c:v>
+                  <c:v>35551.109120679226</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>32863.362920593936</c:v>
+                  <c:v>36465.24391762889</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>33690.7579611564</c:v>
+                  <c:v>37392.61943413657</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>34529.800031719591</c:v>
+                  <c:v>38333.281987245486</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>35380.526563307401</c:v>
+                  <c:v>39287.277558035457</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>36242.974709221147</c:v>
+                  <c:v>40254.651797595696</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>37117.181349992061</c:v>
+                  <c:v>41235.450032829787</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>38003.183098193949</c:v>
+                  <c:v>42229.71727209942</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>38901.016303123186</c:v>
+                  <c:v>43237.498210712416</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>39810.717055349742</c:v>
+                  <c:v>44258.837236262691</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>40732.321191144503</c:v>
+                  <c:v>45293.778433824278</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>41665.864296787899</c:v>
+                  <c:v>46342.365591008471</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>42611.381712763323</c:v>
+                  <c:v>47404.642202887051</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>43568.908537839743</c:v>
+                  <c:v>48480.651476785271</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>44538.47963304841</c:v>
+                  <c:v>49570.436336953186</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>45520.129625555841</c:v>
+                  <c:v>50674.039429114659</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>46513.892912437987</c:v>
+                  <c:v>51791.503124902352</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>47519.803664358595</c:v>
+                  <c:v>52922.869526180657</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>48537.895829154462</c:v>
+                  <c:v>54068.180469260034</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>49568.203135332536</c:v>
+                  <c:v>55227.477529008618</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>50610.759095479203</c:v>
+                  <c:v>56400.802022861862</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>51665.597009587174</c:v>
+                  <c:v>57588.195014735793</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>52732.749968301789</c:v>
+                  <c:v>58789.697318845465</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>53812.250856087659</c:v>
+                  <c:v>60005.349503432903</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>54904.132354322632</c:v>
+                  <c:v>61235.191894406758</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>56008.426944316241</c:v>
+                  <c:v>62479.264578896997</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>57125.166910258566</c:v>
+                  <c:v>63737.607408726588</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>58254.384342100842</c:v>
+                  <c:v>65010.260003803938</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>59396.11113836903</c:v>
+                  <c:v>66297.261755437183</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>60550.379008913755</c:v>
+                  <c:v>67598.651829574344</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>61717.219477598526</c:v>
+                  <c:v>68914.469169970151</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>62896.663884925729</c:v>
+                  <c:v>70244.752501282463</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>64088.743390606833</c:v>
+                  <c:v>71589.540332100762</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>65293.488976073888</c:v>
+                  <c:v>72948.870957908162</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>66510.931446936302</c:v>
+                  <c:v>74322.782463978889</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>67741.101435385339</c:v>
+                  <c:v>75711.312728213496</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>68984.029402546003</c:v>
+                  <c:v>77114.499423914152</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>70239.745640778419</c:v>
+                  <c:v>78532.38002250006</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>71508.280275931145</c:v>
+                  <c:v>79964.991796166636</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>72789.663269546436</c:v>
+                  <c:v>81412.371820488246</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>74083.924421020012</c:v>
+                  <c:v>82874.556976968772</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>75391.093369716007</c:v>
+                  <c:v>84351.58395553779</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>76711.199597037412</c:v>
+                  <c:v>85843.489256997302</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>78044.272428456039</c:v>
+                  <c:v>87350.309195417925</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>79390.341035500373</c:v>
+                  <c:v>88872.079900488709</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>80749.434437702919</c:v>
+                  <c:v>90408.837319817147</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>82121.581504510017</c:v>
+                  <c:v>91960.617221187247</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>83506.810957153197</c:v>
+                  <c:v>93527.455194770126</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>84905.151370483029</c:v>
+                  <c:v>95109.386655293827</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>86316.631174768656</c:v>
+                  <c:v>96706.446844169812</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>87741.278657461356</c:v>
+                  <c:v>98318.670831578958</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>89179.121964924139</c:v>
+                  <c:v>99946.093518517373</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>90630.189104129269</c:v>
+                  <c:v>101588.74963880498</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>92094.50794432321</c:v>
+                  <c:v>103246.67376105444</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>93572.106218658795</c:v>
+                  <c:v>104919.90029060378</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>95063.011525799084</c:v>
+                  <c:v>106608.46347141403</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>96567.251331489941</c:v>
+                  <c:v>108312.39738793176</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>98084.85297010449</c:v>
+                  <c:v>110031.73596691569</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>99615.843646158362</c:v>
+                  <c:v>111766.51297923342</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>101160.25043579798</c:v>
+                  <c:v>113516.7620416218</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>102718.10028826201</c:v>
+                  <c:v>115282.51661842002</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>104289.42002731607</c:v>
+                  <c:v>117063.81002326754</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>105874.23635266184</c:v>
+                  <c:v>118860.67542077569</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>107472.57584132279</c:v>
+                  <c:v>120673.14582816768</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>109084.46494900217</c:v>
+                  <c:v>122501.25411688969</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>110709.93001142096</c:v>
+                  <c:v>124345.03301419674</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>112348.99724563042</c:v>
+                  <c:v>126204.51510470772</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>114001.69275130187</c:v>
+                  <c:v>128079.73283193677</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>115668.04251199565</c:v>
+                  <c:v>129970.71849979584</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>117348.07239640701</c:v>
+                  <c:v>131877.50427407434</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>119041.8081595924</c:v>
+                  <c:v>133800.12218389334</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>120749.27544417309</c:v>
+                  <c:v>135738.60412313321</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>122470.4997815214</c:v>
+                  <c:v>137692.98185184173</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>124205.50659292417</c:v>
+                  <c:v>139663.2869976144</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>125954.32119072901</c:v>
+                  <c:v>141649.55105695577</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>127716.96877947185</c:v>
+                  <c:v>143651.80539661771</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>129493.47445698403</c:v>
+                  <c:v>145670.08125491321</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>131283.86321548402</c:v>
+                  <c:v>147704.40974301344</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>133088.15994264992</c:v>
+                  <c:v>149754.82184622166</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>134906.38942267487</c:v>
+                  <c:v>151821.34842522649</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>136738.57633730577</c:v>
+                  <c:v>153904.02021733596</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>138584.74526686646</c:v>
+                  <c:v>156002.86783769261</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>140444.9206912636</c:v>
+                  <c:v>158117.92178047</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>142319.12699097604</c:v>
+                  <c:v>160249.21242004808</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>144207.38844803252</c:v>
+                  <c:v>162396.77001217374</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>146109.72924696823</c:v>
+                  <c:v>164560.62469510085</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>148026.17347577412</c:v>
+                  <c:v>166740.80649071606</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>149956.74512682288</c:v>
+                  <c:v>168937.34530564255</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>151901.46809778994</c:v>
+                  <c:v>171150.27093233177</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>153860.3661925529</c:v>
+                  <c:v>173379.61305013759</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>155833.46312208218</c:v>
+                  <c:v>175625.40122637275</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>157820.78250531675</c:v>
+                  <c:v>177887.66491735043</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>159822.34787002689</c:v>
+                  <c:v>180166.43346941331</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>161838.18265366266</c:v>
+                  <c:v>182461.73611994152</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>163868.31020419396</c:v>
+                  <c:v>184773.60199835183</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>165912.75378093374</c:v>
+                  <c:v>187102.0601270796</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>167971.53655535154</c:v>
+                  <c:v>189447.13942254533</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>170044.68161187496</c:v>
+                  <c:v>191808.86869610971</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>172132.21194868017</c:v>
+                  <c:v>194187.27665501539</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>174234.15047846915</c:v>
+                  <c:v>196582.39190331142</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>176350.52002923857</c:v>
+                  <c:v>198994.24294276995</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>178481.34334503472</c:v>
+                  <c:v>201422.85817378489</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>180626.64308670099</c:v>
+                  <c:v>203868.26589626307</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>182786.44183261122</c:v>
+                  <c:v>206330.49431049728</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>184960.76207939698</c:v>
+                  <c:v>208809.57151803395</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>187149.62624266159</c:v>
+                  <c:v>211305.52552252213</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>189353.0566576845</c:v>
+                  <c:v>213818.38423055594</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>191571.07558011837</c:v>
+                  <c:v>216348.17545250189</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>193803.7051866735</c:v>
+                  <c:v>218894.92690331896</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>196050.96757579557</c:v>
+                  <c:v>221458.66620336301</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>198312.8847683327</c:v>
+                  <c:v>224039.42087918453</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>200589.4787081934</c:v>
+                  <c:v>226637.21836431159</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>202880.77126299593</c:v>
+                  <c:v>229252.08600002655</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>205186.78422471115</c:v>
+                  <c:v>231884.0510361316</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>207507.53931029388</c:v>
+                  <c:v>234533.14063170063</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>209843.05816230504</c:v>
+                  <c:v>237199.38185582403</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>212193.36234953071</c:v>
+                  <c:v>239882.80168834556</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>214558.47336758795</c:v>
+                  <c:v>242583.42702058743</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>216938.41263952543</c:v>
+                  <c:v>245301.28465606444</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>219333.20151641537</c:v>
+                  <c:v>248036.40131119228</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>221742.86127793801</c:v>
+                  <c:v>250788.8036159848</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>224167.41313295782</c:v>
+                  <c:v>253558.51811474311</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>226606.87822009539</c:v>
+                  <c:v>256345.57126673579</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>229061.27760828673</c:v>
+                  <c:v>259149.98944686979</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>231530.63229734157</c:v>
+                  <c:v>261971.79894635541</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>234014.96321848931</c:v>
+                  <c:v>264811.02597335831</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>236514.29123492076</c:v>
+                  <c:v>267667.69665364822</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>239028.63714232398</c:v>
+                  <c:v>270541.83703123807</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>241558.02166941194</c:v>
+                  <c:v>273433.47306901333</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>244102.46547844275</c:v>
+                  <c:v>276342.6306493553</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>246661.98916573459</c:v>
+                  <c:v>279269.33557475841</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>249236.61326217835</c:v>
+                  <c:v>282213.61356843612</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>251826.35823373467</c:v>
+                  <c:v>285175.49027492345</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>254431.24448193255</c:v>
+                  <c:v>288154.99126066727</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>257051.29234436239</c:v>
+                  <c:v>291152.14201461786</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>259686.52209515605</c:v>
+                  <c:v>294166.96794880333</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>262336.95394546847</c:v>
+                  <c:v>297199.49439890357</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>265002.60804394988</c:v>
+                  <c:v>300249.74662481743</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>267683.50447721384</c:v>
+                  <c:v>303317.74981122091</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>270379.66327029699</c:v>
+                  <c:v>306403.52906811831</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>273091.10438711772</c:v>
+                  <c:v>309507.10943139007</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>275817.84773092705</c:v>
+                  <c:v>312628.51586333197</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>278559.91314475308</c:v>
+                  <c:v>315767.77325318678</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>281317.32041184313</c:v>
+                  <c:v>318924.90641767537</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>284090.08925609681</c:v>
+                  <c:v>322099.94010151358</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>286878.2393425004</c:v>
+                  <c:v>325292.89897793089</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>289681.79027754813</c:v>
+                  <c:v>328503.80764917738</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>292500.76160966698</c:v>
+                  <c:v>331732.69064702984</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>295335.17282962968</c:v>
+                  <c:v>334979.57243328763</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>298185.04337096616</c:v>
+                  <c:v>338244.47740026552</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>301050.39261037199</c:v>
+                  <c:v>341527.42987128237</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>303931.2398681097</c:v>
+                  <c:v>344828.45410113985</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>306827.60440840322</c:v>
+                  <c:v>348147.5742765984</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>309739.5054398374</c:v>
+                  <c:v>351484.81451685331</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>312666.96211573889</c:v>
+                  <c:v>354840.19887399394</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>315609.9935345659</c:v>
+                  <c:v>358213.75133346551</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>318568.61874029005</c:v>
+                  <c:v>361605.49581453012</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>321542.85672276479</c:v>
+                  <c:v>365015.45617071027</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>324532.72641810396</c:v>
+                  <c:v>368443.65619023674</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>327538.24670904857</c:v>
+                  <c:v>371890.11959649331</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>330559.43642532837</c:v>
+                  <c:v>375354.87004844821</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>333596.31434402353</c:v>
+                  <c:v>378837.93114108773</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>336648.89918992063</c:v>
+                  <c:v>382339.32640584133</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>339717.20963586355</c:v>
+                  <c:v>385859.07931100769</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>342801.26430310495</c:v>
+                  <c:v>389397.21326216852</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>345901.08176164894</c:v>
+                  <c:v>392953.75160260574</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>349016.68053059222</c:v>
+                  <c:v>396528.71761370794</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>352148.07907846017</c:v>
+                  <c:v>400122.13451537438</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>355295.295823547</c:v>
+                  <c:v>403734.0254664204</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>358458.34913423873</c:v>
+                  <c:v>407364.41356497019</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>361637.25732934661</c:v>
+                  <c:v>411013.3218488507</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>364832.03867842362</c:v>
+                  <c:v>414680.77329597605</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>368042.71140209428</c:v>
+                  <c:v>418366.79082474136</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>371269.29367236298</c:v>
+                  <c:v>422071.3972943913</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>374511.80361293349</c:v>
+                  <c:v>425794.61550540791</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>377770.25929951732</c:v>
+                  <c:v>429536.46819987474</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>381044.67876014038</c:v>
+                  <c:v>433296.97806185111</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>384335.07997544913</c:v>
+                  <c:v>437076.16771773482</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>387641.48087901168</c:v>
+                  <c:v>440874.05973662593</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>390963.89935761545</c:v>
+                  <c:v>444690.67663068406</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>394302.35325156088</c:v>
+                  <c:v>448526.04085548117</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>397656.86035495787</c:v>
+                  <c:v>452380.17481035594</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>401027.43841601018</c:v>
+                  <c:v>456253.10083875625</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>404414.10513730726</c:v>
+                  <c:v>460144.8412285918</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>407816.87817610218</c:v>
+                  <c:v>464055.41821256437</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>411235.77514459653</c:v>
+                  <c:v>467984.8539685132</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>414670.8136102194</c:v>
+                  <c:v>471933.17061974824</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>418122.01109589828</c:v>
+                  <c:v>475900.39023537457</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>421589.38508033677</c:v>
+                  <c:v>479886.53483062889</c:v>
                 </c:pt>
                 <c:pt idx="280">
-                  <c:v>425072.95299828</c:v>
+                  <c:v>483891.62636719929</c:v>
                 </c:pt>
                 <c:pt idx="281">
-                  <c:v>428572.73224078683</c:v>
+                  <c:v>487915.68675354647</c:v>
                 </c:pt>
                 <c:pt idx="282">
-                  <c:v>432088.74015549204</c:v>
+                  <c:v>491958.73784522427</c:v>
                 </c:pt>
                 <c:pt idx="283">
-                  <c:v>435620.99404686736</c:v>
+                  <c:v>496020.80144519254</c:v>
                 </c:pt>
                 <c:pt idx="284">
-                  <c:v>439169.51117648475</c:v>
+                  <c:v>500101.89930413454</c:v>
                 </c:pt>
                 <c:pt idx="285">
-                  <c:v>442734.308763273</c:v>
+                  <c:v>504202.05312075757</c:v>
                 </c:pt>
                 <c:pt idx="286">
-                  <c:v>446315.40398376866</c:v>
+                  <c:v>508321.28454210883</c:v>
                 </c:pt>
                 <c:pt idx="287">
-                  <c:v>449912.81397237629</c:v>
+                  <c:v>512459.61516387598</c:v>
                 </c:pt>
                 <c:pt idx="288">
-                  <c:v>453526.55582161061</c:v>
+                  <c:v>516617.06653068127</c:v>
                 </c:pt>
                 <c:pt idx="289">
-                  <c:v>457156.64658234856</c:v>
+                  <c:v>520793.66013639153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5345,10 +5345,10 @@
   <dimension ref="A1:N293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="L58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4:N293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5492,7 +5492,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <f>A4^2.3</f>
+        <f>A4^2.323</f>
         <v>0</v>
       </c>
     </row>
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N68" si="2">A5^2.3</f>
+        <f t="shared" ref="N5:N68" si="2">A5^2.323</f>
         <v>1</v>
       </c>
     </row>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>4.9245776533796644</v>
+        <v>5.0037163204530648</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -5652,7 +5652,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>12.513502532843187</v>
+        <v>12.833723394957733</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="N8">
         <f t="shared" si="2"/>
-        <v>24.251465064166357</v>
+        <v>25.037177015568354</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="2"/>
-        <v>40.516414917319047</v>
+        <v>42.044318762978683</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>61.62371493874938</v>
+        <v>64.216311203530324</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>87.846708163528803</v>
+        <v>91.867679574283258</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -5917,7 +5917,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>119.42822291671121</v>
+        <v>125.27893125087172</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>156.58774563947284</v>
+        <v>164.70445617828545</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>199.52623149688802</v>
+        <v>210.37784397664763</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
-        <v>248.42950605272017</v>
+        <v>262.51565509502507</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -6129,7 +6129,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
-        <v>303.47076950560364</v>
+        <v>321.32020440839761</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="2"/>
-        <v>364.81249970724673</v>
+        <v>386.98168153831477</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -6235,7 +6235,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="2"/>
-        <v>432.60793594507902</v>
+        <v>459.67980760799372</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -6288,7 +6288,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="2"/>
-        <v>507.00226068959734</v>
+        <v>539.58515733349998</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="2"/>
-        <v>588.1335577584814</v>
+        <v>626.86023290890432</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>676.13360113393901</v>
+        <v>721.66034956646433</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="2"/>
-        <v>771.12851296924589</v>
+        <v>824.13437543063276</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="2"/>
-        <v>873.2393188170181</v>
+        <v>934.42535671737608</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="2"/>
-        <v>982.58242089263194</v>
+        <v>1052.6710513676792</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -6606,7 +6606,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="2"/>
-        <v>1099.2700051062543</v>
+        <v>1179.0043885929597</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="2"/>
-        <v>1223.4103939473741</v>
+        <v>1313.5538677734057</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -6712,7 +6712,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="2"/>
-        <v>1355.108354635134</v>
+        <v>1456.4439071926699</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="2"/>
-        <v>1494.465369961227</v>
+        <v>1607.7951508896153</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -6818,7 +6818,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="2"/>
-        <v>1641.5798777523532</v>
+        <v>1767.7247402429612</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -6871,7 +6871,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="2"/>
-        <v>1796.5474837318832</v>
+        <v>1936.3465556296376</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
@@ -6924,7 +6924,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="2"/>
-        <v>1959.4611516717455</v>
+        <v>2113.771432509051</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -6977,7 +6977,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="2"/>
-        <v>2130.4113740298362</v>
+        <v>2300.1073555108433</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -7030,7 +7030,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="2"/>
-        <v>2309.4863257178449</v>
+        <v>2495.4596334901012</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -7083,7 +7083,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="2"/>
-        <v>2496.7720032049629</v>
+        <v>2699.931058023868</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="N35">
         <f t="shared" si="2"/>
-        <v>2692.3523508091321</v>
+        <v>2913.6220474276256</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -7191,7 +7191,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="2"/>
-        <v>2896.3093757400966</v>
+        <v>3136.6307780492934</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="N37">
         <f t="shared" si="2"/>
-        <v>3108.7232532236912</v>
+        <v>3369.0533043356754</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="N38">
         <f t="shared" si="2"/>
-        <v>3329.6724228433168</v>
+        <v>3610.9836689495814</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -7356,7 +7356,7 @@
       </c>
       <c r="N39">
         <f t="shared" si="2"/>
-        <v>3559.2336770741695</v>
+        <v>3862.5140040363508</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -7411,7 +7411,7 @@
       </c>
       <c r="N40">
         <f t="shared" si="2"/>
-        <v>3797.4822428522434</v>
+        <v>4123.7346245886538</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="N41">
         <f t="shared" si="2"/>
-        <v>4044.4918569077827</v>
+        <v>4394.7341147325396</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -7521,7 +7521,7 @@
       </c>
       <c r="N42">
         <f t="shared" si="2"/>
-        <v>4300.3348354987693</v>
+        <v>4675.5994076519155</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -7576,7 +7576,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="2"/>
-        <v>4565.0821390994806</v>
+        <v>4966.4158597783535</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="2"/>
-        <v>4838.8034325315484</v>
+        <v>5267.2673197969425</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -7686,7 +7686,7 @@
       </c>
       <c r="N45">
         <f t="shared" si="2"/>
-        <v>5121.5671409661954</v>
+        <v>5578.2361929530007</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -7741,7 +7741,7 @@
       </c>
       <c r="N46">
         <f t="shared" si="2"/>
-        <v>5413.4405021768116</v>
+        <v>5899.403501088379</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -7796,7 +7796,7 @@
       </c>
       <c r="N47">
         <f t="shared" si="2"/>
-        <v>5714.4896153773952</v>
+        <v>6230.8489387876498</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -7851,7 +7851,7 @@
       </c>
       <c r="N48">
         <f t="shared" si="2"/>
-        <v>6024.779486945642</v>
+        <v>6572.6509259720251</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
@@ -7906,7 +7906,7 @@
       </c>
       <c r="N49">
         <f t="shared" si="2"/>
-        <v>6344.3740732964943</v>
+        <v>6924.8866572428878</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
@@ -7961,7 +7961,7 @@
       </c>
       <c r="N50">
         <f t="shared" si="2"/>
-        <v>6673.3363211442738</v>
+        <v>7287.6321482443909</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -8016,7 +8016,7 @@
       </c>
       <c r="N51">
         <f t="shared" si="2"/>
-        <v>7011.7282053664685</v>
+        <v>7660.9622792873633</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
@@ -8071,7 +8071,7 @@
       </c>
       <c r="N52">
         <f t="shared" si="2"/>
-        <v>7359.6107646608343</v>
+        <v>8044.9508364516587</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
@@ -8126,7 +8126,7 @@
       </c>
       <c r="N53">
         <f t="shared" si="2"/>
-        <v>7717.0441351681975</v>
+        <v>8439.6705503631802</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
@@ -8181,7 +8181,7 @@
       </c>
       <c r="N54">
         <f t="shared" si="2"/>
-        <v>8084.0875822169628</v>
+        <v>8845.19313282236</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="N55">
         <f t="shared" si="2"/>
-        <v>8460.7995303299267</v>
+        <v>9261.5893114445098</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
@@ -8291,7 +8291,7 @@
       </c>
       <c r="N56">
         <f t="shared" si="2"/>
-        <v>8847.2375916215024</v>
+        <v>9688.9288624571036</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
@@ -8346,7 +8346,7 @@
       </c>
       <c r="N57">
         <f t="shared" si="2"/>
-        <v>9243.4585927010576</v>
+        <v>10127.280641786332</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="N58">
         <f t="shared" si="2"/>
-        <v>9649.5186001882612</v>
+        <v>10576.712614553002</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
@@ -8456,7 +8456,7 @@
       </c>
       <c r="N59">
         <f t="shared" si="2"/>
-        <v>10065.472944936637</v>
+        <v>11037.291883087411</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
@@ -8511,7 +8511,7 @@
       </c>
       <c r="N60">
         <f t="shared" si="2"/>
-        <v>10491.37624505321</v>
+        <v>11509.084713563765</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
@@ -8566,7 +8566,7 @@
       </c>
       <c r="N61">
         <f t="shared" si="2"/>
-        <v>10927.282427795029</v>
+        <v>11992.156561345526</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="N62">
         <f t="shared" si="2"/>
-        <v>11373.244750415992</v>
+        <v>12486.572095126221</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
@@ -8676,7 +8676,7 @@
       </c>
       <c r="N63">
         <f t="shared" si="2"/>
-        <v>11829.315820032152</v>
+        <v>12992.395219942753</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="N64">
         <f t="shared" si="2"/>
-        <v>12295.547612567134</v>
+        <v>13509.689099132138</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="N65">
         <f t="shared" si="2"/>
-        <v>12771.991490835913</v>
+        <v>14038.516175297907</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
@@ -8841,7 +8841,7 @@
       </c>
       <c r="N66">
         <f t="shared" si="2"/>
-        <v>13258.698221818851</v>
+        <v>14578.938190345483</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
@@ -8896,7 +8896,7 @@
       </c>
       <c r="N67">
         <f t="shared" si="2"/>
-        <v>13755.717993175651</v>
+        <v>15131.016204643307</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
@@ -8951,7 +8951,7 @@
       </c>
       <c r="N68">
         <f t="shared" si="2"/>
-        <v>14263.100429043665</v>
+        <v>15694.810615360644</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
@@ -9005,8 +9005,8 @@
         <v>2851</v>
       </c>
       <c r="N69">
-        <f t="shared" ref="N69:N132" si="27">A69^2.3</f>
-        <v>14780.894605163148</v>
+        <f t="shared" ref="N69:N132" si="27">A69^2.323</f>
+        <v>16270.381174030408</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
@@ -9061,7 +9061,7 @@
       </c>
       <c r="N70">
         <f t="shared" si="27"/>
-        <v>15309.149063367115</v>
+        <v>16857.787003380745</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
@@ -9116,7 +9116,7 @@
       </c>
       <c r="N71">
         <f t="shared" si="27"/>
-        <v>15847.911825473058</v>
+        <v>17457.086613477069</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
@@ -9171,7 +9171,7 @@
       </c>
       <c r="N72">
         <f t="shared" si="27"/>
-        <v>16397.230406608742</v>
+        <v>18068.337917212506</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
@@ -9226,7 +9226,7 @@
       </c>
       <c r="N73">
         <f t="shared" si="27"/>
-        <v>16957.15182800372</v>
+        <v>18691.59824518222</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="N74">
         <f t="shared" si="27"/>
-        <v>17527.72262927581</v>
+        <v>19326.924359975237</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
@@ -9336,7 +9336,7 @@
       </c>
       <c r="N75">
         <f t="shared" si="27"/>
-        <v>18108.988880238638</v>
+        <v>19974.372469914062</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="N76">
         <f t="shared" si="27"/>
-        <v>18700.996192256236</v>
+        <v>20633.998242271638</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
@@ -9446,7 +9446,7 @@
       </c>
       <c r="N77">
         <f t="shared" si="27"/>
-        <v>19303.789729167664</v>
+        <v>21305.856815991738</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
@@ -9501,7 +9501,7 @@
       </c>
       <c r="N78">
         <f t="shared" si="27"/>
-        <v>19917.414217804115</v>
+        <v>21990.0028139391</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
@@ -9556,7 +9556,7 @@
       </c>
       <c r="N79">
         <f t="shared" si="27"/>
-        <v>20541.913958118472</v>
+        <v>22686.490354701677</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
@@ -9611,7 +9611,7 @@
       </c>
       <c r="N80">
         <f t="shared" si="27"/>
-        <v>21177.332832947341</v>
+        <v>23395.373063968567</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
@@ -9666,7 +9666,7 @@
       </c>
       <c r="N81">
         <f t="shared" si="27"/>
-        <v>21823.714317422939</v>
+        <v>24116.704085502843</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="N82">
         <f t="shared" si="27"/>
-        <v>22481.101488051965</v>
+        <v>24850.536091729886</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
@@ -9776,7 +9776,7 @@
       </c>
       <c r="N83">
         <f t="shared" si="27"/>
-        <v>23149.537031478074</v>
+        <v>25596.921293959309</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
@@ -9831,7 +9831,7 @@
       </c>
       <c r="N84">
         <f t="shared" si="27"/>
-        <v>23829.063252941665</v>
+        <v>26355.911452257031</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
@@ -9886,7 +9886,7 @@
       </c>
       <c r="N85">
         <f t="shared" si="27"/>
-        <v>24519.722084452245</v>
+        <v>27127.557884984755</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N86">
         <f t="shared" si="27"/>
-        <v>25221.555092685732</v>
+        <v>27911.911478020902</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
@@ -9996,7 +9996,7 @@
       </c>
       <c r="N87">
         <f t="shared" si="27"/>
-        <v>25934.603486620148</v>
+        <v>28709.022693678744</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
@@ -10051,7 +10051,7 @@
       </c>
       <c r="N88">
         <f t="shared" si="27"/>
-        <v>26658.908124920301</v>
+        <v>29518.94157933387</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
@@ -10106,7 +10106,7 @@
       </c>
       <c r="N89">
         <f t="shared" si="27"/>
-        <v>27394.509523083809</v>
+        <v>30341.717775775051</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
@@ -10161,7 +10161,7 @@
       </c>
       <c r="N90">
         <f t="shared" si="27"/>
-        <v>28141.447860357657</v>
+        <v>31177.40052528942</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="N91">
         <f t="shared" si="27"/>
-        <v>28899.762986436941</v>
+        <v>32026.038679494508</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
@@ -10271,7 +10271,7 @@
       </c>
       <c r="N92">
         <f t="shared" si="27"/>
-        <v>29669.494427952748</v>
+        <v>32887.680706927225</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="N93">
         <f t="shared" si="27"/>
-        <v>30450.681394760803</v>
+        <v>33762.374700399829</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="N94">
         <f t="shared" si="27"/>
-        <v>31243.362786037218</v>
+        <v>34650.168384133904</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
@@ -10436,7 +10436,7 @@
       </c>
       <c r="N95">
         <f t="shared" si="27"/>
-        <v>32047.577196189912</v>
+        <v>35551.109120679226</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="N96">
         <f t="shared" si="27"/>
-        <v>32863.362920593936</v>
+        <v>36465.24391762889</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="N97">
         <f t="shared" si="27"/>
-        <v>33690.7579611564</v>
+        <v>37392.61943413657</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
@@ -10601,7 +10601,7 @@
       </c>
       <c r="N98">
         <f t="shared" si="27"/>
-        <v>34529.800031719591</v>
+        <v>38333.281987245486</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="N99">
         <f t="shared" si="27"/>
-        <v>35380.526563307401</v>
+        <v>39287.277558035457</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
@@ -10711,7 +10711,7 @@
       </c>
       <c r="N100">
         <f t="shared" si="27"/>
-        <v>36242.974709221147</v>
+        <v>40254.651797595696</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
@@ -10766,7 +10766,7 @@
       </c>
       <c r="N101">
         <f t="shared" si="27"/>
-        <v>37117.181349992061</v>
+        <v>41235.450032829787</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
@@ -10821,7 +10821,7 @@
       </c>
       <c r="N102">
         <f t="shared" si="27"/>
-        <v>38003.183098193949</v>
+        <v>42229.71727209942</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
@@ -10876,7 +10876,7 @@
       </c>
       <c r="N103">
         <f t="shared" si="27"/>
-        <v>38901.016303123186</v>
+        <v>43237.498210712416</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
@@ -10931,7 +10931,7 @@
       </c>
       <c r="N104">
         <f t="shared" si="27"/>
-        <v>39810.717055349742</v>
+        <v>44258.837236262691</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="N105">
         <f t="shared" si="27"/>
-        <v>40732.321191144503</v>
+        <v>45293.778433824278</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
@@ -11041,7 +11041,7 @@
       </c>
       <c r="N106">
         <f t="shared" si="27"/>
-        <v>41665.864296787899</v>
+        <v>46342.365591008471</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
@@ -11096,7 +11096,7 @@
       </c>
       <c r="N107">
         <f t="shared" si="27"/>
-        <v>42611.381712763323</v>
+        <v>47404.642202887051</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="N108">
         <f t="shared" si="27"/>
-        <v>43568.908537839743</v>
+        <v>48480.651476785271</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
@@ -11206,7 +11206,7 @@
       </c>
       <c r="N109">
         <f t="shared" si="27"/>
-        <v>44538.47963304841</v>
+        <v>49570.436336953186</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
@@ -11261,7 +11261,7 @@
       </c>
       <c r="N110">
         <f t="shared" si="27"/>
-        <v>45520.129625555841</v>
+        <v>50674.039429114659</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
@@ -11316,7 +11316,7 @@
       </c>
       <c r="N111">
         <f t="shared" si="27"/>
-        <v>46513.892912437987</v>
+        <v>51791.503124902352</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
@@ -11371,7 +11371,7 @@
       </c>
       <c r="N112">
         <f t="shared" si="27"/>
-        <v>47519.803664358595</v>
+        <v>52922.869526180657</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
@@ -11426,7 +11426,7 @@
       </c>
       <c r="N113">
         <f t="shared" si="27"/>
-        <v>48537.895829154462</v>
+        <v>54068.180469260034</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
@@ -11481,7 +11481,7 @@
       </c>
       <c r="N114">
         <f t="shared" si="27"/>
-        <v>49568.203135332536</v>
+        <v>55227.477529008618</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
@@ -11536,7 +11536,7 @@
       </c>
       <c r="N115">
         <f t="shared" si="27"/>
-        <v>50610.759095479203</v>
+        <v>56400.802022861862</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
@@ -11591,7 +11591,7 @@
       </c>
       <c r="N116">
         <f t="shared" si="27"/>
-        <v>51665.597009587174</v>
+        <v>57588.195014735793</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
@@ -11646,7 +11646,7 @@
       </c>
       <c r="N117">
         <f t="shared" si="27"/>
-        <v>52732.749968301789</v>
+        <v>58789.697318845465</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.3">
@@ -11701,7 +11701,7 @@
       </c>
       <c r="N118">
         <f t="shared" si="27"/>
-        <v>53812.250856087659</v>
+        <v>60005.349503432903</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
@@ -11756,7 +11756,7 @@
       </c>
       <c r="N119">
         <f t="shared" si="27"/>
-        <v>54904.132354322632</v>
+        <v>61235.191894406758</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
@@ -11811,7 +11811,7 @@
       </c>
       <c r="N120">
         <f t="shared" si="27"/>
-        <v>56008.426944316241</v>
+        <v>62479.264578896997</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="N121">
         <f t="shared" si="27"/>
-        <v>57125.166910258566</v>
+        <v>63737.607408726588</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
@@ -11921,7 +11921,7 @@
       </c>
       <c r="N122">
         <f t="shared" si="27"/>
-        <v>58254.384342100842</v>
+        <v>65010.260003803938</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
@@ -11976,7 +11976,7 @@
       </c>
       <c r="N123">
         <f t="shared" si="27"/>
-        <v>59396.11113836903</v>
+        <v>66297.261755437183</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
@@ -12031,7 +12031,7 @@
       </c>
       <c r="N124">
         <f t="shared" si="27"/>
-        <v>60550.379008913755</v>
+        <v>67598.651829574344</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
@@ -12086,7 +12086,7 @@
       </c>
       <c r="N125">
         <f t="shared" si="27"/>
-        <v>61717.219477598526</v>
+        <v>68914.469169970151</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
@@ -12141,7 +12141,7 @@
       </c>
       <c r="N126">
         <f t="shared" si="27"/>
-        <v>62896.663884925729</v>
+        <v>70244.752501282463</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
@@ -12196,7 +12196,7 @@
       </c>
       <c r="N127">
         <f t="shared" si="27"/>
-        <v>64088.743390606833</v>
+        <v>71589.540332100762</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.3">
@@ -12251,7 +12251,7 @@
       </c>
       <c r="N128">
         <f t="shared" si="27"/>
-        <v>65293.488976073888</v>
+        <v>72948.870957908162</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.3">
@@ -12306,7 +12306,7 @@
       </c>
       <c r="N129">
         <f t="shared" si="27"/>
-        <v>66510.931446936302</v>
+        <v>74322.782463978889</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.3">
@@ -12361,7 +12361,7 @@
       </c>
       <c r="N130">
         <f t="shared" si="27"/>
-        <v>67741.101435385339</v>
+        <v>75711.312728213496</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
@@ -12416,7 +12416,7 @@
       </c>
       <c r="N131">
         <f t="shared" si="27"/>
-        <v>68984.029402546003</v>
+        <v>77114.499423914152</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.3">
@@ -12471,7 +12471,7 @@
       </c>
       <c r="N132">
         <f t="shared" si="27"/>
-        <v>70239.745640778419</v>
+        <v>78532.38002250006</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.3">
@@ -12525,8 +12525,8 @@
         <v>2851</v>
       </c>
       <c r="N133">
-        <f t="shared" ref="N133:N196" si="38">A133^2.3</f>
-        <v>71508.280275931145</v>
+        <f t="shared" ref="N133:N196" si="38">A133^2.323</f>
+        <v>79964.991796166636</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.3">
@@ -12581,7 +12581,7 @@
       </c>
       <c r="N134">
         <f t="shared" si="38"/>
-        <v>72789.663269546436</v>
+        <v>81412.371820488246</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.3">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="N135">
         <f t="shared" si="38"/>
-        <v>74083.924421020012</v>
+        <v>82874.556976968772</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.3">
@@ -12691,7 +12691,7 @@
       </c>
       <c r="N136">
         <f t="shared" si="38"/>
-        <v>75391.093369716007</v>
+        <v>84351.58395553779</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.3">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="N137">
         <f t="shared" si="38"/>
-        <v>76711.199597037412</v>
+        <v>85843.489256997302</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.3">
@@ -12801,7 +12801,7 @@
       </c>
       <c r="N138">
         <f t="shared" si="38"/>
-        <v>78044.272428456039</v>
+        <v>87350.309195417925</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.3">
@@ -12856,7 +12856,7 @@
       </c>
       <c r="N139">
         <f t="shared" si="38"/>
-        <v>79390.341035500373</v>
+        <v>88872.079900488709</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.3">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="N140">
         <f t="shared" si="38"/>
-        <v>80749.434437702919</v>
+        <v>90408.837319817147</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.3">
@@ -12966,7 +12966,7 @@
       </c>
       <c r="N141">
         <f t="shared" si="38"/>
-        <v>82121.581504510017</v>
+        <v>91960.617221187247</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.3">
@@ -13021,7 +13021,7 @@
       </c>
       <c r="N142">
         <f t="shared" si="38"/>
-        <v>83506.810957153197</v>
+        <v>93527.455194770126</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.3">
@@ -13076,7 +13076,7 @@
       </c>
       <c r="N143">
         <f t="shared" si="38"/>
-        <v>84905.151370483029</v>
+        <v>95109.386655293827</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
@@ -13131,7 +13131,7 @@
       </c>
       <c r="N144">
         <f t="shared" si="38"/>
-        <v>86316.631174768656</v>
+        <v>96706.446844169812</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.3">
@@ -13186,7 +13186,7 @@
       </c>
       <c r="N145">
         <f t="shared" si="38"/>
-        <v>87741.278657461356</v>
+        <v>98318.670831578958</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.3">
@@ -13241,7 +13241,7 @@
       </c>
       <c r="N146">
         <f t="shared" si="38"/>
-        <v>89179.121964924139</v>
+        <v>99946.093518517373</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.3">
@@ -13296,7 +13296,7 @@
       </c>
       <c r="N147">
         <f t="shared" si="38"/>
-        <v>90630.189104129269</v>
+        <v>101588.74963880498</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.3">
@@ -13351,7 +13351,7 @@
       </c>
       <c r="N148">
         <f t="shared" si="38"/>
-        <v>92094.50794432321</v>
+        <v>103246.67376105444</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.3">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="N149">
         <f t="shared" si="38"/>
-        <v>93572.106218658795</v>
+        <v>104919.90029060378</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.3">
@@ -13461,7 +13461,7 @@
       </c>
       <c r="N150">
         <f t="shared" si="38"/>
-        <v>95063.011525799084</v>
+        <v>106608.46347141403</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.3">
@@ -13516,7 +13516,7 @@
       </c>
       <c r="N151">
         <f t="shared" si="38"/>
-        <v>96567.251331489941</v>
+        <v>108312.39738793176</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.3">
@@ -13571,7 +13571,7 @@
       </c>
       <c r="N152">
         <f t="shared" si="38"/>
-        <v>98084.85297010449</v>
+        <v>110031.73596691569</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.3">
@@ -13626,7 +13626,7 @@
       </c>
       <c r="N153">
         <f t="shared" si="38"/>
-        <v>99615.843646158362</v>
+        <v>111766.51297923342</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.3">
@@ -13681,7 +13681,7 @@
       </c>
       <c r="N154">
         <f t="shared" si="38"/>
-        <v>101160.25043579798</v>
+        <v>113516.7620416218</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.3">
@@ -13736,7 +13736,7 @@
       </c>
       <c r="N155">
         <f t="shared" si="38"/>
-        <v>102718.10028826201</v>
+        <v>115282.51661842002</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.3">
@@ -13791,7 +13791,7 @@
       </c>
       <c r="N156">
         <f t="shared" si="38"/>
-        <v>104289.42002731607</v>
+        <v>117063.81002326754</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.3">
@@ -13846,7 +13846,7 @@
       </c>
       <c r="N157">
         <f t="shared" si="38"/>
-        <v>105874.23635266184</v>
+        <v>118860.67542077569</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.3">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="N158">
         <f t="shared" si="38"/>
-        <v>107472.57584132279</v>
+        <v>120673.14582816768</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.3">
@@ -13956,7 +13956,7 @@
       </c>
       <c r="N159">
         <f t="shared" si="38"/>
-        <v>109084.46494900217</v>
+        <v>122501.25411688969</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.3">
@@ -14011,7 +14011,7 @@
       </c>
       <c r="N160">
         <f t="shared" si="38"/>
-        <v>110709.93001142096</v>
+        <v>124345.03301419674</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.3">
@@ -14066,7 +14066,7 @@
       </c>
       <c r="N161">
         <f t="shared" si="38"/>
-        <v>112348.99724563042</v>
+        <v>126204.51510470772</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.3">
@@ -14121,7 +14121,7 @@
       </c>
       <c r="N162">
         <f t="shared" si="38"/>
-        <v>114001.69275130187</v>
+        <v>128079.73283193677</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.3">
@@ -14176,7 +14176,7 @@
       </c>
       <c r="N163">
         <f t="shared" si="38"/>
-        <v>115668.04251199565</v>
+        <v>129970.71849979584</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.3">
@@ -14231,7 +14231,7 @@
       </c>
       <c r="N164">
         <f t="shared" si="38"/>
-        <v>117348.07239640701</v>
+        <v>131877.50427407434</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.3">
@@ -14286,7 +14286,7 @@
       </c>
       <c r="N165">
         <f t="shared" si="38"/>
-        <v>119041.8081595924</v>
+        <v>133800.12218389334</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.3">
@@ -14341,7 +14341,7 @@
       </c>
       <c r="N166">
         <f t="shared" si="38"/>
-        <v>120749.27544417309</v>
+        <v>135738.60412313321</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.3">
@@ -14396,7 +14396,7 @@
       </c>
       <c r="N167">
         <f t="shared" si="38"/>
-        <v>122470.4997815214</v>
+        <v>137692.98185184173</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.3">
@@ -14451,7 +14451,7 @@
       </c>
       <c r="N168">
         <f t="shared" si="38"/>
-        <v>124205.50659292417</v>
+        <v>139663.2869976144</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.3">
@@ -14506,7 +14506,7 @@
       </c>
       <c r="N169">
         <f t="shared" si="38"/>
-        <v>125954.32119072901</v>
+        <v>141649.55105695577</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.3">
@@ -14561,7 +14561,7 @@
       </c>
       <c r="N170">
         <f t="shared" si="38"/>
-        <v>127716.96877947185</v>
+        <v>143651.80539661771</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.3">
@@ -14616,7 +14616,7 @@
       </c>
       <c r="N171">
         <f t="shared" si="38"/>
-        <v>129493.47445698403</v>
+        <v>145670.08125491321</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.3">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="N172">
         <f t="shared" si="38"/>
-        <v>131283.86321548402</v>
+        <v>147704.40974301344</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.3">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="N173">
         <f t="shared" si="38"/>
-        <v>133088.15994264992</v>
+        <v>149754.82184622166</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.3">
@@ -14781,7 +14781,7 @@
       </c>
       <c r="N174">
         <f t="shared" si="38"/>
-        <v>134906.38942267487</v>
+        <v>151821.34842522649</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.3">
@@ -14836,7 +14836,7 @@
       </c>
       <c r="N175">
         <f t="shared" si="38"/>
-        <v>136738.57633730577</v>
+        <v>153904.02021733596</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.3">
@@ -14891,7 +14891,7 @@
       </c>
       <c r="N176">
         <f t="shared" si="38"/>
-        <v>138584.74526686646</v>
+        <v>156002.86783769261</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.3">
@@ -14946,7 +14946,7 @@
       </c>
       <c r="N177">
         <f t="shared" si="38"/>
-        <v>140444.9206912636</v>
+        <v>158117.92178047</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.3">
@@ -15001,7 +15001,7 @@
       </c>
       <c r="N178">
         <f t="shared" si="38"/>
-        <v>142319.12699097604</v>
+        <v>160249.21242004808</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.3">
@@ -15056,7 +15056,7 @@
       </c>
       <c r="N179">
         <f t="shared" si="38"/>
-        <v>144207.38844803252</v>
+        <v>162396.77001217374</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.3">
@@ -15111,7 +15111,7 @@
       </c>
       <c r="N180">
         <f t="shared" si="38"/>
-        <v>146109.72924696823</v>
+        <v>164560.62469510085</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.3">
@@ -15166,7 +15166,7 @@
       </c>
       <c r="N181">
         <f t="shared" si="38"/>
-        <v>148026.17347577412</v>
+        <v>166740.80649071606</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.3">
@@ -15221,7 +15221,7 @@
       </c>
       <c r="N182">
         <f t="shared" si="38"/>
-        <v>149956.74512682288</v>
+        <v>168937.34530564255</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.3">
@@ -15276,7 +15276,7 @@
       </c>
       <c r="N183">
         <f t="shared" si="38"/>
-        <v>151901.46809778994</v>
+        <v>171150.27093233177</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.3">
@@ -15331,7 +15331,7 @@
       </c>
       <c r="N184">
         <f t="shared" si="38"/>
-        <v>153860.3661925529</v>
+        <v>173379.61305013759</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.3">
@@ -15386,7 +15386,7 @@
       </c>
       <c r="N185">
         <f t="shared" si="38"/>
-        <v>155833.46312208218</v>
+        <v>175625.40122637275</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.3">
@@ -15441,7 +15441,7 @@
       </c>
       <c r="N186">
         <f t="shared" si="38"/>
-        <v>157820.78250531675</v>
+        <v>177887.66491735043</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.3">
@@ -15496,7 +15496,7 @@
       </c>
       <c r="N187">
         <f t="shared" si="38"/>
-        <v>159822.34787002689</v>
+        <v>180166.43346941331</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.3">
@@ -15551,7 +15551,7 @@
       </c>
       <c r="N188">
         <f t="shared" si="38"/>
-        <v>161838.18265366266</v>
+        <v>182461.73611994152</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.3">
@@ -15606,7 +15606,7 @@
       </c>
       <c r="N189">
         <f t="shared" si="38"/>
-        <v>163868.31020419396</v>
+        <v>184773.60199835183</v>
       </c>
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.3">
@@ -15661,7 +15661,7 @@
       </c>
       <c r="N190">
         <f t="shared" si="38"/>
-        <v>165912.75378093374</v>
+        <v>187102.0601270796</v>
       </c>
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.3">
@@ -15716,7 +15716,7 @@
       </c>
       <c r="N191">
         <f t="shared" si="38"/>
-        <v>167971.53655535154</v>
+        <v>189447.13942254533</v>
       </c>
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.3">
@@ -15771,7 +15771,7 @@
       </c>
       <c r="N192">
         <f t="shared" si="38"/>
-        <v>170044.68161187496</v>
+        <v>191808.86869610971</v>
       </c>
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.3">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="N193">
         <f t="shared" si="38"/>
-        <v>172132.21194868017</v>
+        <v>194187.27665501539</v>
       </c>
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.3">
@@ -15881,7 +15881,7 @@
       </c>
       <c r="N194">
         <f t="shared" si="38"/>
-        <v>174234.15047846915</v>
+        <v>196582.39190331142</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.3">
@@ -15936,7 +15936,7 @@
       </c>
       <c r="N195">
         <f t="shared" si="38"/>
-        <v>176350.52002923857</v>
+        <v>198994.24294276995</v>
       </c>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.3">
@@ -15991,7 +15991,7 @@
       </c>
       <c r="N196">
         <f t="shared" si="38"/>
-        <v>178481.34334503472</v>
+        <v>201422.85817378489</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.3">
@@ -16045,8 +16045,8 @@
         <v>2851</v>
       </c>
       <c r="N197">
-        <f t="shared" ref="N197:N260" si="49">A197^2.3</f>
-        <v>180626.64308670099</v>
+        <f t="shared" ref="N197:N260" si="49">A197^2.323</f>
+        <v>203868.26589626307</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.3">
@@ -16101,7 +16101,7 @@
       </c>
       <c r="N198">
         <f t="shared" si="49"/>
-        <v>182786.44183261122</v>
+        <v>206330.49431049728</v>
       </c>
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.3">
@@ -16156,7 +16156,7 @@
       </c>
       <c r="N199">
         <f t="shared" si="49"/>
-        <v>184960.76207939698</v>
+        <v>208809.57151803395</v>
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.3">
@@ -16211,7 +16211,7 @@
       </c>
       <c r="N200">
         <f t="shared" si="49"/>
-        <v>187149.62624266159</v>
+        <v>211305.52552252213</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.3">
@@ -16266,7 +16266,7 @@
       </c>
       <c r="N201">
         <f t="shared" si="49"/>
-        <v>189353.0566576845</v>
+        <v>213818.38423055594</v>
       </c>
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.3">
@@ -16321,7 +16321,7 @@
       </c>
       <c r="N202">
         <f t="shared" si="49"/>
-        <v>191571.07558011837</v>
+        <v>216348.17545250189</v>
       </c>
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.3">
@@ -16376,7 +16376,7 @@
       </c>
       <c r="N203">
         <f t="shared" si="49"/>
-        <v>193803.7051866735</v>
+        <v>218894.92690331896</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.3">
@@ -16431,7 +16431,7 @@
       </c>
       <c r="N204">
         <f t="shared" si="49"/>
-        <v>196050.96757579557</v>
+        <v>221458.66620336301</v>
       </c>
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.3">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="N205">
         <f t="shared" si="49"/>
-        <v>198312.8847683327</v>
+        <v>224039.42087918453</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.3">
@@ -16541,7 +16541,7 @@
       </c>
       <c r="N206">
         <f t="shared" si="49"/>
-        <v>200589.4787081934</v>
+        <v>226637.21836431159</v>
       </c>
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.3">
@@ -16596,7 +16596,7 @@
       </c>
       <c r="N207">
         <f t="shared" si="49"/>
-        <v>202880.77126299593</v>
+        <v>229252.08600002655</v>
       </c>
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.3">
@@ -16651,7 +16651,7 @@
       </c>
       <c r="N208">
         <f t="shared" si="49"/>
-        <v>205186.78422471115</v>
+        <v>231884.0510361316</v>
       </c>
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.3">
@@ -16706,7 +16706,7 @@
       </c>
       <c r="N209">
         <f t="shared" si="49"/>
-        <v>207507.53931029388</v>
+        <v>234533.14063170063</v>
       </c>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
@@ -16761,7 +16761,7 @@
       </c>
       <c r="N210">
         <f t="shared" si="49"/>
-        <v>209843.05816230504</v>
+        <v>237199.38185582403</v>
       </c>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
@@ -16816,7 +16816,7 @@
       </c>
       <c r="N211">
         <f t="shared" si="49"/>
-        <v>212193.36234953071</v>
+        <v>239882.80168834556</v>
       </c>
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.3">
@@ -16871,7 +16871,7 @@
       </c>
       <c r="N212">
         <f t="shared" si="49"/>
-        <v>214558.47336758795</v>
+        <v>242583.42702058743</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.3">
@@ -16926,7 +16926,7 @@
       </c>
       <c r="N213">
         <f t="shared" si="49"/>
-        <v>216938.41263952543</v>
+        <v>245301.28465606444</v>
       </c>
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.3">
@@ -16981,7 +16981,7 @@
       </c>
       <c r="N214">
         <f t="shared" si="49"/>
-        <v>219333.20151641537</v>
+        <v>248036.40131119228</v>
       </c>
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.3">
@@ -17036,7 +17036,7 @@
       </c>
       <c r="N215">
         <f t="shared" si="49"/>
-        <v>221742.86127793801</v>
+        <v>250788.8036159848</v>
       </c>
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.3">
@@ -17091,7 +17091,7 @@
       </c>
       <c r="N216">
         <f t="shared" si="49"/>
-        <v>224167.41313295782</v>
+        <v>253558.51811474311</v>
       </c>
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.3">
@@ -17146,7 +17146,7 @@
       </c>
       <c r="N217">
         <f t="shared" si="49"/>
-        <v>226606.87822009539</v>
+        <v>256345.57126673579</v>
       </c>
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.3">
@@ -17201,7 +17201,7 @@
       </c>
       <c r="N218">
         <f t="shared" si="49"/>
-        <v>229061.27760828673</v>
+        <v>259149.98944686979</v>
       </c>
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.3">
@@ -17256,7 +17256,7 @@
       </c>
       <c r="N219">
         <f t="shared" si="49"/>
-        <v>231530.63229734157</v>
+        <v>261971.79894635541</v>
       </c>
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.3">
@@ -17311,7 +17311,7 @@
       </c>
       <c r="N220">
         <f t="shared" si="49"/>
-        <v>234014.96321848931</v>
+        <v>264811.02597335831</v>
       </c>
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.3">
@@ -17366,7 +17366,7 @@
       </c>
       <c r="N221">
         <f t="shared" si="49"/>
-        <v>236514.29123492076</v>
+        <v>267667.69665364822</v>
       </c>
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.3">
@@ -17421,7 +17421,7 @@
       </c>
       <c r="N222">
         <f t="shared" si="49"/>
-        <v>239028.63714232398</v>
+        <v>270541.83703123807</v>
       </c>
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.3">
@@ -17476,7 +17476,7 @@
       </c>
       <c r="N223">
         <f t="shared" si="49"/>
-        <v>241558.02166941194</v>
+        <v>273433.47306901333</v>
       </c>
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.3">
@@ -17531,7 +17531,7 @@
       </c>
       <c r="N224">
         <f t="shared" si="49"/>
-        <v>244102.46547844275</v>
+        <v>276342.6306493553</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.3">
@@ -17586,7 +17586,7 @@
       </c>
       <c r="N225">
         <f t="shared" si="49"/>
-        <v>246661.98916573459</v>
+        <v>279269.33557475841</v>
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.3">
@@ -17641,7 +17641,7 @@
       </c>
       <c r="N226">
         <f t="shared" si="49"/>
-        <v>249236.61326217835</v>
+        <v>282213.61356843612</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.3">
@@ -17696,7 +17696,7 @@
       </c>
       <c r="N227">
         <f t="shared" si="49"/>
-        <v>251826.35823373467</v>
+        <v>285175.49027492345</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.3">
@@ -17751,7 +17751,7 @@
       </c>
       <c r="N228">
         <f t="shared" si="49"/>
-        <v>254431.24448193255</v>
+        <v>288154.99126066727</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.3">
@@ -17806,7 +17806,7 @@
       </c>
       <c r="N229">
         <f t="shared" si="49"/>
-        <v>257051.29234436239</v>
+        <v>291152.14201461786</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.3">
@@ -17861,7 +17861,7 @@
       </c>
       <c r="N230">
         <f t="shared" si="49"/>
-        <v>259686.52209515605</v>
+        <v>294166.96794880333</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.3">
@@ -17916,7 +17916,7 @@
       </c>
       <c r="N231">
         <f t="shared" si="49"/>
-        <v>262336.95394546847</v>
+        <v>297199.49439890357</v>
       </c>
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.3">
@@ -17971,7 +17971,7 @@
       </c>
       <c r="N232">
         <f t="shared" si="49"/>
-        <v>265002.60804394988</v>
+        <v>300249.74662481743</v>
       </c>
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.3">
@@ -18026,7 +18026,7 @@
       </c>
       <c r="N233">
         <f t="shared" si="49"/>
-        <v>267683.50447721384</v>
+        <v>303317.74981122091</v>
       </c>
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.3">
@@ -18081,7 +18081,7 @@
       </c>
       <c r="N234">
         <f t="shared" si="49"/>
-        <v>270379.66327029699</v>
+        <v>306403.52906811831</v>
       </c>
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.3">
@@ -18136,7 +18136,7 @@
       </c>
       <c r="N235">
         <f t="shared" si="49"/>
-        <v>273091.10438711772</v>
+        <v>309507.10943139007</v>
       </c>
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.3">
@@ -18191,7 +18191,7 @@
       </c>
       <c r="N236">
         <f t="shared" si="49"/>
-        <v>275817.84773092705</v>
+        <v>312628.51586333197</v>
       </c>
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.3">
@@ -18246,7 +18246,7 @@
       </c>
       <c r="N237">
         <f t="shared" si="49"/>
-        <v>278559.91314475308</v>
+        <v>315767.77325318678</v>
       </c>
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.3">
@@ -18301,7 +18301,7 @@
       </c>
       <c r="N238">
         <f t="shared" si="49"/>
-        <v>281317.32041184313</v>
+        <v>318924.90641767537</v>
       </c>
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.3">
@@ -18356,7 +18356,7 @@
       </c>
       <c r="N239">
         <f t="shared" si="49"/>
-        <v>284090.08925609681</v>
+        <v>322099.94010151358</v>
       </c>
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.3">
@@ -18411,7 +18411,7 @@
       </c>
       <c r="N240">
         <f t="shared" si="49"/>
-        <v>286878.2393425004</v>
+        <v>325292.89897793089</v>
       </c>
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.3">
@@ -18466,7 +18466,7 @@
       </c>
       <c r="N241">
         <f t="shared" si="49"/>
-        <v>289681.79027754813</v>
+        <v>328503.80764917738</v>
       </c>
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.3">
@@ -18521,7 +18521,7 @@
       </c>
       <c r="N242">
         <f t="shared" si="49"/>
-        <v>292500.76160966698</v>
+        <v>331732.69064702984</v>
       </c>
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.3">
@@ -18576,7 +18576,7 @@
       </c>
       <c r="N243">
         <f t="shared" si="49"/>
-        <v>295335.17282962968</v>
+        <v>334979.57243328763</v>
       </c>
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.3">
@@ -18631,7 +18631,7 @@
       </c>
       <c r="N244">
         <f t="shared" si="49"/>
-        <v>298185.04337096616</v>
+        <v>338244.47740026552</v>
       </c>
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.3">
@@ -18686,7 +18686,7 @@
       </c>
       <c r="N245">
         <f t="shared" si="49"/>
-        <v>301050.39261037199</v>
+        <v>341527.42987128237</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.3">
@@ -18741,7 +18741,7 @@
       </c>
       <c r="N246">
         <f t="shared" si="49"/>
-        <v>303931.2398681097</v>
+        <v>344828.45410113985</v>
       </c>
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.3">
@@ -18796,7 +18796,7 @@
       </c>
       <c r="N247">
         <f t="shared" si="49"/>
-        <v>306827.60440840322</v>
+        <v>348147.5742765984</v>
       </c>
     </row>
     <row r="248" spans="1:14" x14ac:dyDescent="0.3">
@@ -18851,7 +18851,7 @@
       </c>
       <c r="N248">
         <f t="shared" si="49"/>
-        <v>309739.5054398374</v>
+        <v>351484.81451685331</v>
       </c>
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.3">
@@ -18906,7 +18906,7 @@
       </c>
       <c r="N249">
         <f t="shared" si="49"/>
-        <v>312666.96211573889</v>
+        <v>354840.19887399394</v>
       </c>
     </row>
     <row r="250" spans="1:14" x14ac:dyDescent="0.3">
@@ -18961,7 +18961,7 @@
       </c>
       <c r="N250">
         <f t="shared" si="49"/>
-        <v>315609.9935345659</v>
+        <v>358213.75133346551</v>
       </c>
     </row>
     <row r="251" spans="1:14" x14ac:dyDescent="0.3">
@@ -19016,7 +19016,7 @@
       </c>
       <c r="N251">
         <f t="shared" si="49"/>
-        <v>318568.61874029005</v>
+        <v>361605.49581453012</v>
       </c>
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.3">
@@ -19071,7 +19071,7 @@
       </c>
       <c r="N252">
         <f t="shared" si="49"/>
-        <v>321542.85672276479</v>
+        <v>365015.45617071027</v>
       </c>
     </row>
     <row r="253" spans="1:14" x14ac:dyDescent="0.3">
@@ -19126,7 +19126,7 @@
       </c>
       <c r="N253">
         <f t="shared" si="49"/>
-        <v>324532.72641810396</v>
+        <v>368443.65619023674</v>
       </c>
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.3">
@@ -19181,7 +19181,7 @@
       </c>
       <c r="N254">
         <f t="shared" si="49"/>
-        <v>327538.24670904857</v>
+        <v>371890.11959649331</v>
       </c>
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.3">
@@ -19236,7 +19236,7 @@
       </c>
       <c r="N255">
         <f t="shared" si="49"/>
-        <v>330559.43642532837</v>
+        <v>375354.87004844821</v>
       </c>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.3">
@@ -19291,7 +19291,7 @@
       </c>
       <c r="N256">
         <f t="shared" si="49"/>
-        <v>333596.31434402353</v>
+        <v>378837.93114108773</v>
       </c>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.3">
@@ -19346,7 +19346,7 @@
       </c>
       <c r="N257">
         <f t="shared" si="49"/>
-        <v>336648.89918992063</v>
+        <v>382339.32640584133</v>
       </c>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.3">
@@ -19401,7 +19401,7 @@
       </c>
       <c r="N258">
         <f t="shared" si="49"/>
-        <v>339717.20963586355</v>
+        <v>385859.07931100769</v>
       </c>
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.3">
@@ -19456,7 +19456,7 @@
       </c>
       <c r="N259">
         <f t="shared" si="49"/>
-        <v>342801.26430310495</v>
+        <v>389397.21326216852</v>
       </c>
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.3">
@@ -19511,7 +19511,7 @@
       </c>
       <c r="N260">
         <f t="shared" si="49"/>
-        <v>345901.08176164894</v>
+        <v>392953.75160260574</v>
       </c>
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.3">
@@ -19565,8 +19565,8 @@
         <v>2851</v>
       </c>
       <c r="N261">
-        <f t="shared" ref="N261:N293" si="60">A261^2.3</f>
-        <v>349016.68053059222</v>
+        <f t="shared" ref="N261:N293" si="60">A261^2.323</f>
+        <v>396528.71761370794</v>
       </c>
     </row>
     <row r="262" spans="1:14" x14ac:dyDescent="0.3">
@@ -19621,7 +19621,7 @@
       </c>
       <c r="N262">
         <f t="shared" si="60"/>
-        <v>352148.07907846017</v>
+        <v>400122.13451537438</v>
       </c>
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.3">
@@ -19676,7 +19676,7 @@
       </c>
       <c r="N263">
         <f t="shared" si="60"/>
-        <v>355295.295823547</v>
+        <v>403734.0254664204</v>
       </c>
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.3">
@@ -19731,7 +19731,7 @@
       </c>
       <c r="N264">
         <f t="shared" si="60"/>
-        <v>358458.34913423873</v>
+        <v>407364.41356497019</v>
       </c>
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.3">
@@ -19786,7 +19786,7 @@
       </c>
       <c r="N265">
         <f t="shared" si="60"/>
-        <v>361637.25732934661</v>
+        <v>411013.3218488507</v>
       </c>
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.3">
@@ -19841,7 +19841,7 @@
       </c>
       <c r="N266">
         <f t="shared" si="60"/>
-        <v>364832.03867842362</v>
+        <v>414680.77329597605</v>
       </c>
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.3">
@@ -19896,7 +19896,7 @@
       </c>
       <c r="N267">
         <f t="shared" si="60"/>
-        <v>368042.71140209428</v>
+        <v>418366.79082474136</v>
       </c>
     </row>
     <row r="268" spans="1:14" x14ac:dyDescent="0.3">
@@ -19951,7 +19951,7 @@
       </c>
       <c r="N268">
         <f t="shared" si="60"/>
-        <v>371269.29367236298</v>
+        <v>422071.3972943913</v>
       </c>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.3">
@@ -20006,7 +20006,7 @@
       </c>
       <c r="N269">
         <f t="shared" si="60"/>
-        <v>374511.80361293349</v>
+        <v>425794.61550540791</v>
       </c>
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.3">
@@ -20061,7 +20061,7 @@
       </c>
       <c r="N270">
         <f t="shared" si="60"/>
-        <v>377770.25929951732</v>
+        <v>429536.46819987474</v>
       </c>
     </row>
     <row r="271" spans="1:14" x14ac:dyDescent="0.3">
@@ -20116,7 +20116,7 @@
       </c>
       <c r="N271">
         <f t="shared" si="60"/>
-        <v>381044.67876014038</v>
+        <v>433296.97806185111</v>
       </c>
     </row>
     <row r="272" spans="1:14" x14ac:dyDescent="0.3">
@@ -20171,7 +20171,7 @@
       </c>
       <c r="N272">
         <f t="shared" si="60"/>
-        <v>384335.07997544913</v>
+        <v>437076.16771773482</v>
       </c>
     </row>
     <row r="273" spans="1:14" x14ac:dyDescent="0.3">
@@ -20226,7 +20226,7 @@
       </c>
       <c r="N273">
         <f t="shared" si="60"/>
-        <v>387641.48087901168</v>
+        <v>440874.05973662593</v>
       </c>
     </row>
     <row r="274" spans="1:14" x14ac:dyDescent="0.3">
@@ -20281,7 +20281,7 @@
       </c>
       <c r="N274">
         <f t="shared" si="60"/>
-        <v>390963.89935761545</v>
+        <v>444690.67663068406</v>
       </c>
     </row>
     <row r="275" spans="1:14" x14ac:dyDescent="0.3">
@@ -20336,7 +20336,7 @@
       </c>
       <c r="N275">
         <f t="shared" si="60"/>
-        <v>394302.35325156088</v>
+        <v>448526.04085548117</v>
       </c>
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.3">
@@ -20391,7 +20391,7 @@
       </c>
       <c r="N276">
         <f t="shared" si="60"/>
-        <v>397656.86035495787</v>
+        <v>452380.17481035594</v>
       </c>
     </row>
     <row r="277" spans="1:14" x14ac:dyDescent="0.3">
@@ -20446,7 +20446,7 @@
       </c>
       <c r="N277">
         <f t="shared" si="60"/>
-        <v>401027.43841601018</v>
+        <v>456253.10083875625</v>
       </c>
     </row>
     <row r="278" spans="1:14" x14ac:dyDescent="0.3">
@@ -20501,7 +20501,7 @@
       </c>
       <c r="N278">
         <f t="shared" si="60"/>
-        <v>404414.10513730726</v>
+        <v>460144.8412285918</v>
       </c>
     </row>
     <row r="279" spans="1:14" x14ac:dyDescent="0.3">
@@ -20556,7 +20556,7 @@
       </c>
       <c r="N279">
         <f t="shared" si="60"/>
-        <v>407816.87817610218</v>
+        <v>464055.41821256437</v>
       </c>
     </row>
     <row r="280" spans="1:14" x14ac:dyDescent="0.3">
@@ -20611,7 +20611,7 @@
       </c>
       <c r="N280">
         <f t="shared" si="60"/>
-        <v>411235.77514459653</v>
+        <v>467984.8539685132</v>
       </c>
     </row>
     <row r="281" spans="1:14" x14ac:dyDescent="0.3">
@@ -20666,7 +20666,7 @@
       </c>
       <c r="N281">
         <f t="shared" si="60"/>
-        <v>414670.8136102194</v>
+        <v>471933.17061974824</v>
       </c>
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.3">
@@ -20721,7 +20721,7 @@
       </c>
       <c r="N282">
         <f t="shared" si="60"/>
-        <v>418122.01109589828</v>
+        <v>475900.39023537457</v>
       </c>
     </row>
     <row r="283" spans="1:14" x14ac:dyDescent="0.3">
@@ -20776,7 +20776,7 @@
       </c>
       <c r="N283">
         <f t="shared" si="60"/>
-        <v>421589.38508033677</v>
+        <v>479886.53483062889</v>
       </c>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.3">
@@ -20831,7 +20831,7 @@
       </c>
       <c r="N284">
         <f t="shared" si="60"/>
-        <v>425072.95299828</v>
+        <v>483891.62636719929</v>
       </c>
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.3">
@@ -20886,7 +20886,7 @@
       </c>
       <c r="N285">
         <f t="shared" si="60"/>
-        <v>428572.73224078683</v>
+        <v>487915.68675354647</v>
       </c>
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.3">
@@ -20941,7 +20941,7 @@
       </c>
       <c r="N286">
         <f t="shared" si="60"/>
-        <v>432088.74015549204</v>
+        <v>491958.73784522427</v>
       </c>
     </row>
     <row r="287" spans="1:14" x14ac:dyDescent="0.3">
@@ -20996,7 +20996,7 @@
       </c>
       <c r="N287">
         <f t="shared" si="60"/>
-        <v>435620.99404686736</v>
+        <v>496020.80144519254</v>
       </c>
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.3">
@@ -21051,7 +21051,7 @@
       </c>
       <c r="N288">
         <f t="shared" si="60"/>
-        <v>439169.51117648475</v>
+        <v>500101.89930413454</v>
       </c>
     </row>
     <row r="289" spans="1:14" x14ac:dyDescent="0.3">
@@ -21106,7 +21106,7 @@
       </c>
       <c r="N289">
         <f t="shared" si="60"/>
-        <v>442734.308763273</v>
+        <v>504202.05312075757</v>
       </c>
     </row>
     <row r="290" spans="1:14" x14ac:dyDescent="0.3">
@@ -21161,7 +21161,7 @@
       </c>
       <c r="N290">
         <f t="shared" si="60"/>
-        <v>446315.40398376866</v>
+        <v>508321.28454210883</v>
       </c>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.3">
@@ -21216,7 +21216,7 @@
       </c>
       <c r="N291">
         <f t="shared" si="60"/>
-        <v>449912.81397237629</v>
+        <v>512459.61516387598</v>
       </c>
     </row>
     <row r="292" spans="1:14" x14ac:dyDescent="0.3">
@@ -21271,7 +21271,7 @@
       </c>
       <c r="N292">
         <f t="shared" si="60"/>
-        <v>453526.55582161061</v>
+        <v>516617.06653068127</v>
       </c>
     </row>
     <row r="293" spans="1:14" x14ac:dyDescent="0.3">
@@ -21326,7 +21326,7 @@
       </c>
       <c r="N293">
         <f t="shared" si="60"/>
-        <v>457156.64658234856</v>
+        <v>520793.66013639153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>